<commit_message>
Workspaces and template for rewritten Basic Desktop Ch4 exercises
</commit_message>
<xml_diff>
--- a/Resources/DesktopBasic/AddressSchema.xlsx
+++ b/Resources/DesktopBasic/AddressSchema.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Number</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Event</t>
+  </si>
+  <si>
+    <t>Owners</t>
   </si>
 </sst>
 </file>
@@ -376,51 +379,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="40.7109375" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="64.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="64.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>